<commit_message>
add loan due date
</commit_message>
<xml_diff>
--- a/account-withdraw.xlsx
+++ b/account-withdraw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Date" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
   <si>
     <t>账单日</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>28日</t>
+  </si>
+  <si>
+    <t>农业银行</t>
   </si>
   <si>
     <t>29日</t>
@@ -136,17 +139,40 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -159,6 +185,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -166,90 +214,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,9 +282,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,16 +298,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,19 +314,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +476,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,151 +494,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,45 +505,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -547,6 +519,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,11 +549,50 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,15 +605,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -602,10 +613,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -614,142 +625,145 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1073,7 +1087,7 @@
   <dimension ref="D1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:Q10"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1366,6 +1380,9 @@
       <c r="D30" t="s">
         <v>33</v>
       </c>
+      <c r="K30" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="Q30" t="s">
         <v>33</v>
       </c>
@@ -1374,32 +1391,35 @@
       <c r="D31" t="s">
         <v>34</v>
       </c>
+      <c r="K31" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="Q31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="4:17">
       <c r="D32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="4:17">
       <c r="D33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="4:17">
       <c r="D34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
collect data of applying cards
</commit_message>
<xml_diff>
--- a/account-withdraw.xlsx
+++ b/account-withdraw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="16965" windowHeight="12630" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Date" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
   <si>
     <t>起刷日</t>
   </si>
@@ -90,12 +90,12 @@
     <t>14日</t>
   </si>
   <si>
+    <t>民生银行</t>
+  </si>
+  <si>
     <t>15日</t>
   </si>
   <si>
-    <t>民生银行</t>
-  </si>
-  <si>
     <t>16日</t>
   </si>
   <si>
@@ -150,16 +150,16 @@
     <t>卡</t>
   </si>
   <si>
-    <t>下卡日期</t>
-  </si>
-  <si>
-    <t>二卡下卡日期</t>
-  </si>
-  <si>
-    <t>三卡</t>
-  </si>
-  <si>
-    <t>四卡</t>
+    <t>首申日期</t>
+  </si>
+  <si>
+    <t>渠道/结果</t>
+  </si>
+  <si>
+    <t>材料</t>
+  </si>
+  <si>
+    <t>开卡日期</t>
   </si>
   <si>
     <t>当前额度</t>
@@ -168,28 +168,128 @@
     <t>原始额度</t>
   </si>
   <si>
-    <t>日期</t>
+    <t>提额日期</t>
+  </si>
+  <si>
+    <t>额度</t>
   </si>
   <si>
     <t>提额原因</t>
   </si>
   <si>
-    <t>额度</t>
+    <t>二卡日期</t>
+  </si>
+  <si>
+    <t>上门/成功</t>
+  </si>
+  <si>
+    <t>工牌</t>
   </si>
   <si>
     <t>第一次25个月提额</t>
+  </si>
+  <si>
+    <t>网申/成功</t>
+  </si>
+  <si>
+    <t>无</t>
+  </si>
+  <si>
+    <t>无(房贷，不需要面签)</t>
+  </si>
+  <si>
+    <t>无（网点开卡遇麻烦）</t>
+  </si>
+  <si>
+    <t>无（5分钟出额度）</t>
+  </si>
+  <si>
+    <t>网点/成功</t>
+  </si>
+  <si>
+    <t>双证</t>
+  </si>
+  <si>
+    <t>双证+收入证明</t>
+  </si>
+  <si>
+    <t>无（芝麻信用781）</t>
+  </si>
+  <si>
+    <t>兴业银行</t>
+  </si>
+  <si>
+    <t>网点</t>
+  </si>
+  <si>
+    <t>上海银行</t>
+  </si>
+  <si>
+    <t>行驶证+收入证明+农行信用卡</t>
+  </si>
+  <si>
+    <t>平安银行</t>
+  </si>
+  <si>
+    <t>网申</t>
+  </si>
+  <si>
+    <t>无（行驶证，大堂经理手机操作）</t>
+  </si>
+  <si>
+    <t>邮储银行</t>
+  </si>
+  <si>
+    <t>上门</t>
+  </si>
+  <si>
+    <t>双证+公积金(支付宝)+工牌</t>
+  </si>
+  <si>
+    <t>浙商银行</t>
+  </si>
+  <si>
+    <t>双证+公积金(支付宝)+收入证明+光大信用卡</t>
+  </si>
+  <si>
+    <t>华夏银行</t>
+  </si>
+  <si>
+    <t>无（小白信用98.9，白条15k，金条20k）</t>
+  </si>
+  <si>
+    <t>工商银行</t>
+  </si>
+  <si>
+    <t>花旗银行</t>
+  </si>
+  <si>
+    <t>汇丰银行</t>
+  </si>
+  <si>
+    <t>温州银行</t>
+  </si>
+  <si>
+    <t>宁波银行</t>
+  </si>
+  <si>
+    <t>浦发银行</t>
+  </si>
+  <si>
+    <t>杭州银行</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -208,29 +308,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -239,16 +316,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,14 +339,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,7 +354,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,21 +363,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,17 +378,54 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -345,8 +437,16 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,18 +461,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -385,7 +605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,151 +617,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,6 +652,56 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -579,32 +729,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,182 +752,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -809,13 +909,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -824,7 +924,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1149,7 +1249,7 @@
   <dimension ref="B1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1173,8 +1273,8 @@
       <c r="L1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="5:15">
       <c r="E2" s="5"/>
@@ -1185,8 +1285,8 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="6"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" spans="5:15">
       <c r="E3" s="5"/>
@@ -1197,8 +1297,8 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="6"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="5:12">
       <c r="E4" t="s">
@@ -1353,6 +1453,9 @@
       <c r="F17" t="s">
         <v>14</v>
       </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
       <c r="L17" t="s">
         <v>23</v>
       </c>
@@ -1362,13 +1465,10 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" t="s">
         <v>25</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:12">
@@ -1499,7 +1599,7 @@
         <v>36</v>
       </c>
       <c r="F28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L28" t="s">
         <v>36</v>
@@ -1526,7 +1626,7 @@
       <c r="E30" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L30" t="s">
@@ -1540,7 +1640,7 @@
       <c r="E31" t="s">
         <v>39</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L31" t="s">
@@ -1643,25 +1743,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="5.875" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="2" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="37.25" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="15.625" customWidth="1"/>
-    <col min="10" max="10" width="6.625" customWidth="1"/>
-    <col min="11" max="11" width="12.125" customWidth="1"/>
-    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.625" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="10.625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1677,7 +1776,7 @@
       <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1686,7 +1785,7 @@
       <c r="G1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I1" t="s">
@@ -1695,227 +1794,367 @@
       <c r="J1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" t="s">
-        <v>50</v>
+      <c r="K1" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
+        <v>42227</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2">
         <v>42241</v>
       </c>
-      <c r="C2" s="4">
-        <v>42956</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
       <c r="F2">
         <v>35</v>
       </c>
       <c r="G2">
         <v>25</v>
       </c>
-      <c r="H2" s="4">
-        <v>42241</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="2">
+        <v>42998</v>
+      </c>
+      <c r="I2">
         <v>35</v>
       </c>
-      <c r="K2" s="4">
-        <v>42998</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="2">
+        <v>42956</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
+        <v>42957</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2">
         <v>42965</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
       <c r="F3">
         <v>40</v>
       </c>
       <c r="G3">
         <v>40</v>
       </c>
-      <c r="H3" s="4">
-        <v>42965</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
+        <v>42957</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="2">
         <v>42965</v>
       </c>
-      <c r="E4" s="4"/>
       <c r="F4">
         <v>9.7</v>
       </c>
       <c r="G4">
         <v>9.7</v>
       </c>
-      <c r="H4" s="4">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2">
         <v>42965</v>
       </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="C5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42982</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42969</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="2">
         <v>42980</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5">
+      <c r="F6">
         <v>15</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>15</v>
       </c>
-      <c r="H5" s="4">
-        <v>42980</v>
-      </c>
-      <c r="I5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4">
-        <v>42982</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" s="4">
-        <v>42982</v>
-      </c>
-      <c r="I6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
+        <v>42985</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="2">
         <v>42996</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
       <c r="F7">
         <v>10</v>
       </c>
       <c r="G7">
         <v>10</v>
       </c>
-      <c r="H7" s="4">
-        <v>42996</v>
-      </c>
-      <c r="I7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
+        <v>42985</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="2">
         <v>42999</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
       <c r="F8">
         <v>40</v>
       </c>
       <c r="G8">
         <v>40</v>
       </c>
-      <c r="H8" s="4">
-        <v>42999</v>
-      </c>
-      <c r="I8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>42986</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2">
+        <v>43014</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="2">
+        <v>42990</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2">
         <v>43000</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9">
+      <c r="F10">
         <v>50</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>50</v>
       </c>
-      <c r="H9" s="4">
-        <v>43000</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4">
-        <v>43014</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10">
-        <v>20</v>
-      </c>
-      <c r="G10">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4">
-        <v>43014</v>
-      </c>
-      <c r="I10" t="s">
-        <v>49</v>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2">
+        <v>42998</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43001</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43003</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43017</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43018</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43018</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of credit cards info
</commit_message>
<xml_diff>
--- a/account-withdraw.xlsx
+++ b/account-withdraw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19350" windowHeight="12630"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Date" sheetId="2" r:id="rId1"/>
@@ -38,93 +38,93 @@
     <t>3日</t>
   </si>
   <si>
+    <t>4日</t>
+  </si>
+  <si>
+    <t>5日</t>
+  </si>
+  <si>
+    <t>6日</t>
+  </si>
+  <si>
+    <t>光大银行</t>
+  </si>
+  <si>
+    <t>招商银行</t>
+  </si>
+  <si>
+    <t>7日</t>
+  </si>
+  <si>
+    <t>华夏银行</t>
+  </si>
+  <si>
+    <t>农业银行</t>
+  </si>
+  <si>
+    <t>8日</t>
+  </si>
+  <si>
+    <t>中信银行</t>
+  </si>
+  <si>
+    <t>中国银行</t>
+  </si>
+  <si>
+    <t>9日</t>
+  </si>
+  <si>
+    <t>上海银行</t>
+  </si>
+  <si>
+    <t>10日</t>
+  </si>
+  <si>
+    <t>11日</t>
+  </si>
+  <si>
+    <t>12日</t>
+  </si>
+  <si>
+    <t>13日</t>
+  </si>
+  <si>
+    <t>民生银行</t>
+  </si>
+  <si>
+    <t>14日</t>
+  </si>
+  <si>
+    <t>15日</t>
+  </si>
+  <si>
+    <t>交通银行</t>
+  </si>
+  <si>
+    <t>16日</t>
+  </si>
+  <si>
+    <t>17日</t>
+  </si>
+  <si>
+    <t>18日</t>
+  </si>
+  <si>
+    <t>19日</t>
+  </si>
+  <si>
+    <t>20日</t>
+  </si>
+  <si>
+    <t>21日</t>
+  </si>
+  <si>
+    <t>22日</t>
+  </si>
+  <si>
     <t>建设银行</t>
   </si>
   <si>
-    <t>4日</t>
-  </si>
-  <si>
-    <t>5日</t>
-  </si>
-  <si>
-    <t>6日</t>
-  </si>
-  <si>
-    <t>光大银行</t>
-  </si>
-  <si>
-    <t>招商银行</t>
-  </si>
-  <si>
-    <t>7日</t>
-  </si>
-  <si>
-    <t>华夏银行</t>
-  </si>
-  <si>
-    <t>农业银行</t>
-  </si>
-  <si>
-    <t>8日</t>
-  </si>
-  <si>
-    <t>中信银行</t>
-  </si>
-  <si>
-    <t>中国银行</t>
-  </si>
-  <si>
-    <t>9日</t>
-  </si>
-  <si>
-    <t>10日</t>
-  </si>
-  <si>
-    <t>上海银行</t>
-  </si>
-  <si>
-    <t>11日</t>
-  </si>
-  <si>
-    <t>12日</t>
-  </si>
-  <si>
-    <t>13日</t>
-  </si>
-  <si>
-    <t>14日</t>
-  </si>
-  <si>
-    <t>民生银行</t>
-  </si>
-  <si>
-    <t>15日</t>
-  </si>
-  <si>
-    <t>16日</t>
-  </si>
-  <si>
-    <t>交通银行</t>
-  </si>
-  <si>
-    <t>17日</t>
-  </si>
-  <si>
-    <t>18日</t>
-  </si>
-  <si>
-    <t>19日</t>
-  </si>
-  <si>
-    <t>20日</t>
-  </si>
-  <si>
-    <t>21日</t>
-  </si>
-  <si>
-    <t>22日</t>
-  </si>
-  <si>
     <t>23日</t>
   </si>
   <si>
@@ -158,7 +158,7 @@
     <t>2.加粗为不能修改账单日</t>
   </si>
   <si>
-    <t>3.绿色为起刷日和账单日相同</t>
+    <t>3.下划线为起刷日和账单日不同</t>
   </si>
   <si>
     <t>4.斜体为56天</t>
@@ -529,12 +529,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -553,16 +553,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -584,19 +586,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -607,38 +600,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -659,9 +630,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -677,7 +677,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,38 +714,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -750,7 +752,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,25 +788,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,25 +896,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,109 +926,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -944,11 +946,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,21 +976,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -992,17 +985,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1025,8 +1012,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1046,148 +1048,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1567,7 +1569,7 @@
   <dimension ref="B1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1629,7 +1631,7 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="L5" t="s">
@@ -1640,41 +1642,40 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
       <c r="L6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="5:12">
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F7" s="11"/>
       <c r="L7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="5:12">
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F8" s="11"/>
       <c r="L8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="5:13">
       <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="K9" t="s">
         <v>10</v>
       </c>
-      <c r="K9" t="s">
-        <v>11</v>
-      </c>
       <c r="L9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M9">
         <v>35</v>
@@ -1682,16 +1683,16 @@
     </row>
     <row r="10" spans="5:13">
       <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s">
+      <c r="K10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="14" t="s">
-        <v>14</v>
-      </c>
       <c r="L10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M10">
         <v>40</v>
@@ -1702,47 +1703,49 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
+      <c r="K11" t="s">
         <v>16</v>
       </c>
-      <c r="K11" t="s">
-        <v>17</v>
-      </c>
       <c r="L11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:13">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="K12" s="14" t="s">
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="F13" s="11"/>
       <c r="L13" t="s">
         <v>19</v>
-      </c>
-      <c r="M13">
-        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:12">
@@ -1750,10 +1753,11 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F14" s="11"/>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -1761,72 +1765,74 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F15" s="11"/>
       <c r="L15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="K16" t="s">
         <v>23</v>
       </c>
       <c r="L16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
+        <v>22</v>
+      </c>
+      <c r="M16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" t="s">
-        <v>25</v>
+      <c r="F17" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="L17" t="s">
         <v>24</v>
       </c>
-      <c r="M17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
       <c r="L18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
+        <v>25</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="L19" t="s">
         <v>27</v>
-      </c>
-      <c r="M19">
-        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:12">
@@ -1834,10 +1840,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:12">
@@ -1845,16 +1851,16 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -1862,10 +1868,12 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
       <c r="L22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -1873,10 +1881,12 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
       <c r="L23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:13">
@@ -1884,13 +1894,15 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
       <c r="K24" t="s">
         <v>4</v>
       </c>
       <c r="L24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M24">
         <v>40</v>
@@ -1901,16 +1913,17 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="K25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K25" t="s">
-        <v>6</v>
-      </c>
       <c r="L25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M25">
         <v>10</v>
@@ -1935,7 +1948,7 @@
         <v>36</v>
       </c>
       <c r="K27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L27" t="s">
         <v>36</v>
@@ -1944,40 +1957,43 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:13">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" t="s">
         <v>37</v>
       </c>
-      <c r="F28" t="s">
-        <v>25</v>
+      <c r="F28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
+        <v>12</v>
       </c>
       <c r="L28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="2:14">
+      <c r="M28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" t="s">
         <v>38</v>
       </c>
-      <c r="J29" t="s">
-        <v>13</v>
+      <c r="F29" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="K29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L29" t="s">
         <v>38</v>
       </c>
       <c r="M29">
-        <v>30</v>
-      </c>
-      <c r="N29">
         <v>20</v>
       </c>
     </row>
@@ -1989,7 +2005,7 @@
         <v>39</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L30" t="s">
         <v>39</v>
@@ -2003,7 +2019,7 @@
         <v>40</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L31" t="s">
         <v>40</v>
@@ -2182,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>59</v>
@@ -2287,7 +2303,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>68</v>
@@ -2325,7 +2341,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>70</v>
@@ -2364,7 +2380,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>73</v>
@@ -2403,12 +2419,11 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
         <v>76</v>
       </c>
@@ -2462,12 +2477,11 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>76</v>
       </c>
@@ -2499,12 +2513,11 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>65</v>
       </c>
@@ -2536,12 +2549,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
         <v>61</v>
       </c>
@@ -2594,12 +2606,11 @@
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
         <v>71</v>
       </c>
@@ -2635,7 +2646,6 @@
       <c r="C15" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
         <v>61</v>
       </c>
@@ -2697,7 +2707,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
         <v>103</v>
@@ -2899,7 +2909,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5">
         <v>42241</v>
@@ -2956,7 +2966,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5">
         <v>42965</v>
@@ -2967,7 +2977,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5">
         <v>42980</v>
@@ -2978,7 +2988,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5">
         <v>42982</v>
@@ -2989,7 +2999,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5">
         <v>42996</v>
@@ -3000,7 +3010,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5">
         <v>42999</v>
@@ -3011,7 +3021,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5">
         <v>43000</v>
@@ -3022,7 +3032,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5">
         <v>43014</v>
@@ -3033,7 +3043,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5">
         <v>43024</v>
@@ -3044,7 +3054,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
         <v>43026</v>
@@ -3065,7 +3075,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3169,7 +3179,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -3227,7 +3237,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -3244,7 +3254,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -3261,7 +3271,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>35</v>
@@ -3278,7 +3288,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="J8">
         <v>23</v>
@@ -3295,7 +3305,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9">
         <v>6</v>
@@ -3312,7 +3322,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -3329,7 +3339,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -3346,12 +3356,12 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>